<commit_message>
Fixing position header in forms 3BU
</commit_message>
<xml_diff>
--- a/forms/Form-3BU-multiple.xlsx
+++ b/forms/Form-3BU-multiple.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED38CC67-550E-42E1-A9E6-500A70B65E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D478283E-5255-4CFA-9175-95134734F3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="GFpj//VivYAPeIU08ZJg1Dux9toxRhSuIx/DIcXzwdN7RVpS32MIopnBIf/zfwa+hDKrfFh8CXTLPmmG/7iI6w==" workbookSaltValue="5rYiPYrZuKGJOy5hPiufCQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>Position at 12:00 GMT</t>
-  </si>
-  <si>
     <t>Original data</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>3-BU-multiple</t>
+  </si>
+  <si>
+    <t>Buoy position</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1205,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="45"/>
       <c r="F4" s="43" t="s">
@@ -1530,10 +1530,10 @@
       <c r="D4" s="70"/>
       <c r="E4" s="71"/>
       <c r="F4" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="67" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" s="68"/>
     </row>
@@ -1551,7 +1551,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="52" t="s">
         <v>25</v>
@@ -2011,7 +2011,7 @@
       <c r="H55" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DFw7S0Z+jnsiLLFL/0DFd9N6tohQqJjAO2uvMqDdyKey+ocBWJn9kNCImB6vGkk5IuxH1RwoAkSA9D3qnqA3Qw==" saltValue="g2CoM840SFt4dWK3QRA9vQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lh0RyzXA4zLC5+CQ2xOwdPLh7mRqxC6gSPscJEP1kN7SPup/7c9fnkNt5Xe9aPIxf6M7YRQDdeyqEGWaQvF9gg==" saltValue="79bI4YlCKRmHKHcmEF6D5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="G4:H4"/>

</xml_diff>